<commit_message>
Results from October_25,_2020--23:17:44 run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-10-25.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-10-25.xlsx
@@ -605,21 +605,39 @@
           <t>North Carolina</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="B5" s="2" t="n">
+        <v>44129</v>
+      </c>
+      <c r="C5" t="n">
+        <v>260099</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4157</v>
+      </c>
+      <c r="E5" t="n">
+        <v>47548</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1184</v>
+      </c>
+      <c r="G5" t="n">
+        <v>22.74</v>
+      </c>
+      <c r="H5" t="n">
+        <v>29.94</v>
+      </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>209101</v>
+      </c>
+      <c r="L5" t="n">
+        <v>3954</v>
+      </c>
       <c r="M5" t="n">
         <v>2179622</v>
       </c>
@@ -628,7 +646,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -661,7 +679,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... KeyError('SUM(# probable)')</t>
         </is>
       </c>
     </row>
@@ -690,7 +708,7 @@
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>
@@ -880,7 +898,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... KeyError("None of ['Categories'] are in the columns")</t>
         </is>
       </c>
     </row>
@@ -960,7 +978,7 @@
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'text'")</t>
         </is>
       </c>
     </row>
@@ -1036,21 +1054,39 @@
           <t>Maryland</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="B16" s="2" t="n">
+        <v>44129</v>
+      </c>
+      <c r="C16" t="n">
+        <v>140279</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3950</v>
+      </c>
+      <c r="E16" t="n">
+        <v>43513</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1606</v>
+      </c>
+      <c r="G16" t="n">
+        <v>36.45</v>
+      </c>
+      <c r="H16" t="n">
+        <v>40.78</v>
+      </c>
       <c r="I16" t="b">
         <v>0</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
       </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
+      <c r="K16" t="n">
+        <v>119377</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3938</v>
+      </c>
       <c r="M16" t="n">
         <v>1788090</v>
       </c>
@@ -1059,7 +1095,7 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1230,7 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... JSONDecodeError('Expecting value: line 1 column 1 (char 0)')</t>
         </is>
       </c>
     </row>
@@ -1331,21 +1367,41 @@
           <t>Oklahoma</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2020-10-25</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>116736</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1249</v>
+      </c>
+      <c r="E23" t="n">
+        <v>8031.4368</v>
+      </c>
+      <c r="F23" t="n">
+        <v>80.0609</v>
+      </c>
+      <c r="G23" t="n">
+        <v>6.88</v>
+      </c>
+      <c r="H23" t="n">
+        <v>6.41</v>
+      </c>
       <c r="I23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="b">
         <v>0</v>
       </c>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
+      <c r="K23" t="n">
+        <v>95151.51360000001</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1157.9479</v>
+      </c>
       <c r="M23" t="n">
         <v>287959</v>
       </c>
@@ -1354,7 +1410,7 @@
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -1430,7 +1486,7 @@
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>
@@ -1643,18 +1699,32 @@
           <t>Iowa</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
+      <c r="B31" s="2" t="n">
+        <v>44130</v>
+      </c>
+      <c r="C31" t="n">
+        <v>116238</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1635</v>
+      </c>
+      <c r="E31" t="n">
+        <v>5488</v>
+      </c>
+      <c r="F31" t="n">
+        <v>57</v>
+      </c>
+      <c r="G31" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="H31" t="n">
+        <v>3.49</v>
+      </c>
       <c r="I31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
@@ -1666,7 +1736,7 @@
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -1904,7 +1974,7 @@
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>
@@ -1984,7 +2054,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... NoSuchElementException('no such element: Unable to locate element: {"method":"xpath","selector":"//a[@data-chart-id=\'count-charts\']"}\n  (Session info: headless chrome=86.0.4240.111)', None, None)</t>
         </is>
       </c>
     </row>
@@ -2115,7 +2185,7 @@
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>
@@ -2332,7 +2402,7 @@
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>
@@ -2467,7 +2537,7 @@
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>
@@ -2510,21 +2580,39 @@
           <t>Arizona</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
+      <c r="B52" s="2" t="n">
+        <v>44129</v>
+      </c>
+      <c r="C52" t="n">
+        <v>238163</v>
+      </c>
+      <c r="D52" t="n">
+        <v>5874</v>
+      </c>
+      <c r="E52" t="n">
+        <v>7371</v>
+      </c>
+      <c r="F52" t="n">
+        <v>181</v>
+      </c>
+      <c r="G52" t="n">
+        <v>4.39</v>
+      </c>
+      <c r="H52" t="n">
+        <v>3.46</v>
+      </c>
       <c r="I52" t="b">
         <v>0</v>
       </c>
       <c r="J52" t="b">
         <v>0</v>
       </c>
-      <c r="K52" t="inlineStr"/>
-      <c r="L52" t="inlineStr"/>
+      <c r="K52" t="n">
+        <v>167906</v>
+      </c>
+      <c r="L52" t="n">
+        <v>5235</v>
+      </c>
       <c r="M52" t="n">
         <v>305259</v>
       </c>
@@ -2533,7 +2621,7 @@
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -2642,7 +2730,7 @@
       <c r="N55" t="inlineStr"/>
       <c r="O55" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>
@@ -2699,21 +2787,39 @@
           <t>New Hampshire</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
+      <c r="B57" s="2" t="n">
+        <v>44129</v>
+      </c>
+      <c r="C57" t="n">
+        <v>10328</v>
+      </c>
+      <c r="D57" t="n">
+        <v>473</v>
+      </c>
+      <c r="E57" t="n">
+        <v>408</v>
+      </c>
+      <c r="F57" t="n">
+        <v>9</v>
+      </c>
+      <c r="G57" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="H57" t="n">
+        <v>1.99</v>
+      </c>
       <c r="I57" t="b">
         <v>0</v>
       </c>
       <c r="J57" t="b">
         <v>0</v>
       </c>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr"/>
+      <c r="K57" t="n">
+        <v>8964</v>
+      </c>
+      <c r="L57" t="n">
+        <v>452</v>
+      </c>
       <c r="M57" t="n">
         <v>20516</v>
       </c>
@@ -2722,7 +2828,7 @@
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>An error occurred. ... SessionNotCreatedException('session not created: This version of ChromeDriver only supports Chrome version 83', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>